<commit_message>
Sync NSGA folder from VS Code (code, data, results)
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yueru/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93CE7CF-7EA6-3C45-9508-7802444C16FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C43BFED-4AEB-554E-914E-C69407507399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6065" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6065" uniqueCount="160">
   <si>
     <t>EnglishName</t>
   </si>
@@ -507,12 +507,20 @@
   <si>
     <t>Timetable sheet contains many missing FirstDepartureHour/Headway; your code infers headway=168/frequency and fd=0 when missing.</t>
   </si>
+  <si>
+    <t>https://www.climatiq.io/data/emission-factor/c38f802d-2c43-4123-ab62-5f5468f503fd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.climatiq.io/data/emission-factor/0ae70778-80a9-409f-9c3f-44a277cee752</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +542,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -552,15 +568,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -862,8 +881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A38" sqref="A38:E40"/>
     </sheetView>
   </sheetViews>
@@ -4642,17 +4661,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N712"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A689" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A710" sqref="A710:XFD712"/>
+      <selection pane="bottomLeft" activeCell="E689" sqref="E689"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -35506,7 +35525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -35670,7 +35689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="163" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -35967,7 +35986,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -36195,8 +36214,8 @@
       <c r="E11" t="s">
         <v>110</v>
       </c>
-      <c r="F11" t="s">
-        <v>111</v>
+      <c r="F11" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -36235,8 +36254,8 @@
       <c r="E13" t="s">
         <v>112</v>
       </c>
-      <c r="F13" t="s">
-        <v>113</v>
+      <c r="F13" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -36301,6 +36320,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1" xr:uid="{28476BB4-931F-3345-AB5F-0DA919F78F06}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{88848255-23A5-024C-A5E2-77E88AFBFA9B}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>